<commit_message>
[Dipto] refactor: Sending mail to a person in the AddressBook by name
</commit_message>
<xml_diff>
--- a/AddressBookTable.xlsx
+++ b/AddressBookTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UI Path\Projects\AddressBookUiPathProblem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21A6F55C-147E-45B3-93A4-FCFC6BD1AB4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5594BBA3-0003-46D7-92BA-C25E67AEF92D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{A344445D-43BC-431C-B220-40B213AFF8B8}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>